<commit_message>
Made addScheduleMaterial and updateScheduleMaterial more effecient by using switch case statements
</commit_message>
<xml_diff>
--- a/server/template.xlsx
+++ b/server/template.xlsx
@@ -72,13 +72,39 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Bookman Old Style"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,20 +124,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -389,119 +425,140 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A10:I19"/>
+  <dimension ref="A10:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="7.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.109375" customWidth="1"/>
     <col min="3" max="3" width="9.44140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="10" spans="1:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+    <row r="10" spans="1:10" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:9" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="17" spans="1:9" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="17" spans="1:10" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A17:I17"/>
-    <mergeCell ref="C10:G10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
+  <mergeCells count="11">
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A17:J17"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="C11:G11"/>
+    <mergeCell ref="C15:J15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:E12"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="C14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>